<commit_message>
updated homepage complete (including excel documentation)
</commit_message>
<xml_diff>
--- a/Template+SEO+analysis.xlsx
+++ b/Template+SEO+analysis.xlsx
@@ -1,38 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colin.meldrum/Library/Containers/com.microsoft.Excel/Data/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Documents\GitHub\OC_P4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4A3739EF-62A6-7A47-B5E8-326C4BE794FA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E899FEE-D623-499D-8E00-ED4B209B88B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15940" xr2:uid="{F4D0CAC2-2123-1946-879C-AB8072365C64}"/>
+    <workbookView xWindow="-4780" yWindow="2720" windowWidth="10120" windowHeight="8920" xr2:uid="{F4D0CAC2-2123-1946-879C-AB8072365C64}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="69">
   <si>
     <t>Explanation</t>
   </si>
@@ -49,10 +42,196 @@
     <t>Issue analyzed</t>
   </si>
   <si>
-    <t>(SEO or Accessibility?)</t>
-  </si>
-  <si>
     <t>Action recommended</t>
+  </si>
+  <si>
+    <t>SEO</t>
+  </si>
+  <si>
+    <t>fail</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>Title tag should be 70 characters and indicate the topic of the page to search engines. It must include the target keyword and make visitors want to click and read the page.</t>
+  </si>
+  <si>
+    <t>Change title to "GoMikeDesigns - Freelance Web Designer Atlanta"</t>
+  </si>
+  <si>
+    <t>Change description content to "Hire an Atlanta-based website and graphic design agency to make business attractive and recognizable online."</t>
+  </si>
+  <si>
+    <t>keywords meta</t>
+  </si>
+  <si>
+    <t>description meta</t>
+  </si>
+  <si>
+    <t>Description meta should be around 160 characters and indicate the topic of the page to search engines. It must include the target keyword and make visitors want to click and read the page.</t>
+  </si>
+  <si>
+    <t>Delete tag</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>scripts</t>
+  </si>
+  <si>
+    <t>Script tags should be placed within the body tag (after DOM).</t>
+  </si>
+  <si>
+    <t>Keywords meta no longer used by search engines.</t>
+  </si>
+  <si>
+    <t>Move tags to body</t>
+  </si>
+  <si>
+    <t>stylesheets</t>
+  </si>
+  <si>
+    <t>analytics</t>
+  </si>
+  <si>
+    <t>Install Google Analytics and Google Search Console.</t>
+  </si>
+  <si>
+    <t>No Google analytics tag on the website.</t>
+  </si>
+  <si>
+    <t>black hat SEO techniques</t>
+  </si>
+  <si>
+    <t>Remove hidden text containing keywords.</t>
+  </si>
+  <si>
+    <t>SEO, accessibility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accessibility </t>
+  </si>
+  <si>
+    <t>navbar</t>
+  </si>
+  <si>
+    <t>Black hat SEO techniques are punished by Google.</t>
+  </si>
+  <si>
+    <t>CSS files should be linked in the head.</t>
+  </si>
+  <si>
+    <t>Empty li tag.</t>
+  </si>
+  <si>
+    <t>img alt</t>
+  </si>
+  <si>
+    <t>Alt for cartoon image of mike contains keywords instead of description.</t>
+  </si>
+  <si>
+    <t>Change alt to "cartoon picture of Mike"</t>
+  </si>
+  <si>
+    <t>h1</t>
+  </si>
+  <si>
+    <t>Multiple h1 tags, main h1 tag does not contain keywords.</t>
+  </si>
+  <si>
+    <t>change subsection headings to h2 tags, change main h1 tag to "I'm Mike, a freelance web designer based in Atlanta."</t>
+  </si>
+  <si>
+    <t>bloc-1-hero background</t>
+  </si>
+  <si>
+    <t>Low contrast, image contains text.</t>
+  </si>
+  <si>
+    <t>remove the following classes "bgc-dark-slate-blue bg-atlanta-20made-20sign".</t>
+  </si>
+  <si>
+    <t>bloc-2-services title</t>
+  </si>
+  <si>
+    <t>Should be h2 tag not image.</t>
+  </si>
+  <si>
+    <t>Delete img and replace with h2 tag.</t>
+  </si>
+  <si>
+    <t>service headers</t>
+  </si>
+  <si>
+    <t>The should only be one h1 tag on page.</t>
+  </si>
+  <si>
+    <t>Replace h1s with h2 tags.</t>
+  </si>
+  <si>
+    <t>testimonial</t>
+  </si>
+  <si>
+    <t>Image with text is not accessible or responsive.</t>
+  </si>
+  <si>
+    <t>replace with em, strong, and p tags that contain text.</t>
+  </si>
+  <si>
+    <t>service description text</t>
+  </si>
+  <si>
+    <t>Text is too small.</t>
+  </si>
+  <si>
+    <t>Replace with h5 tags.</t>
+  </si>
+  <si>
+    <t>bloc-3-what-i-do</t>
+  </si>
+  <si>
+    <t>bloc-3-what-i-do text</t>
+  </si>
+  <si>
+    <t>Text is hard to read due to low contrast and noisy background image</t>
+  </si>
+  <si>
+    <t>Text is too repetitive.</t>
+  </si>
+  <si>
+    <t>Remove the following classes "bg-atlanta-20made-20sign-20orange bgc-atomic-tangerine". Remove "black-background" class from text container div.</t>
+  </si>
+  <si>
+    <t>Remove text.</t>
+  </si>
+  <si>
+    <t>bloc-3-what-i-do contact me link</t>
+  </si>
+  <si>
+    <t>For the best UX, the link should be a button that is centered and colorful.</t>
+  </si>
+  <si>
+    <t>Add the following classes to the link "btn btn-lg btn-clean btn-rd cta-hero btn-atomic-tangerine", add the class of "text-center" to parent element of link.</t>
+  </si>
+  <si>
+    <t>bloc-4-portfolio header</t>
+  </si>
+  <si>
+    <t>Put image text into an h2 and delete image.</t>
+  </si>
+  <si>
+    <t>bloc-5-cta</t>
+  </si>
+  <si>
+    <t>footer</t>
+  </si>
+  <si>
+    <t>Remove row containing links to partners and directories.</t>
+  </si>
+  <si>
+    <t>Contains lots of links that are irrelevant to users. They could also be interpreted by Google as blackhat SEO techniques.</t>
   </si>
 </sst>
 </file>
@@ -134,7 +313,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -430,13 +609,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21008D1C-867F-FF4D-8036-BD2682FF7900}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" customWidth="1"/>
@@ -445,7 +624,7 @@
     <col min="6" max="6" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -459,18 +638,368 @@
         <v>0</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" t="s">
+        <v>68</v>
+      </c>
+      <c r="E22" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
contact page + compressed images + new lighthouse report
</commit_message>
<xml_diff>
--- a/Template+SEO+analysis.xlsx
+++ b/Template+SEO+analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Documents\GitHub\OC_P4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E899FEE-D623-499D-8E00-ED4B209B88B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E808D49C-E4B3-4CEF-B455-38C259DE2256}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4780" yWindow="2720" windowWidth="10120" windowHeight="8920" xr2:uid="{F4D0CAC2-2123-1946-879C-AB8072365C64}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="97">
   <si>
     <t>Explanation</t>
   </si>
@@ -232,6 +232,90 @@
   </si>
   <si>
     <t>Contains lots of links that are irrelevant to users. They could also be interpreted by Google as blackhat SEO techniques.</t>
+  </si>
+  <si>
+    <t>page2.html</t>
+  </si>
+  <si>
+    <t>Filename will not create a descriptive url.</t>
+  </si>
+  <si>
+    <t>Rename file as "contact.html" and change links that point towards it.</t>
+  </si>
+  <si>
+    <t>Change description content to "Contact Mike, a freelance web developer based in Atlanta."</t>
+  </si>
+  <si>
+    <t>SEO, accessibility, performance</t>
+  </si>
+  <si>
+    <t>Contact page html links to stylesheets that are not available.</t>
+  </si>
+  <si>
+    <t>Contact page contains scripts that are not working properly or area unavailable</t>
+  </si>
+  <si>
+    <t>Replace scripts with those used for the homepage.</t>
+  </si>
+  <si>
+    <t>Replace stylesheet links with those that are used for the homepage.</t>
+  </si>
+  <si>
+    <t>contact block-6</t>
+  </si>
+  <si>
+    <t>Low contrast text.</t>
+  </si>
+  <si>
+    <t>Remove class "bgc-dark-slate-blue" from container div.</t>
+  </si>
+  <si>
+    <t>Heading uses p tag.</t>
+  </si>
+  <si>
+    <t>Replace with p tag with h1 tag.</t>
+  </si>
+  <si>
+    <t>Replace p tag with h4 tag.</t>
+  </si>
+  <si>
+    <t>Supporting paragraph text is too small.</t>
+  </si>
+  <si>
+    <t>robots meta tag</t>
+  </si>
+  <si>
+    <t>Add robots meta tag to index.html and set content to "index, follow".</t>
+  </si>
+  <si>
+    <t>No robots meta tag to help search engines index the website.</t>
+  </si>
+  <si>
+    <t>logo</t>
+  </si>
+  <si>
+    <t>Logo img alt attribute contains keywords, a black hat SEO technique.</t>
+  </si>
+  <si>
+    <t>Replace alt contents with "logo".</t>
+  </si>
+  <si>
+    <t>portfolio images</t>
+  </si>
+  <si>
+    <t>Image files are very big and contain keywords in alt attribute.</t>
+  </si>
+  <si>
+    <t>lang</t>
+  </si>
+  <si>
+    <t>"Default" is not a valid value for this attribute.</t>
+  </si>
+  <si>
+    <t>Replace with "en".</t>
+  </si>
+  <si>
+    <t>Downsize (compress) images and replace alt attributes with relevant descriptions.</t>
   </si>
 </sst>
 </file>
@@ -609,10 +693,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21008D1C-867F-FF4D-8036-BD2682FF7900}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="E14" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -998,6 +1082,193 @@
         <v>67</v>
       </c>
     </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" t="s">
+        <v>70</v>
+      </c>
+      <c r="E23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" t="s">
+        <v>74</v>
+      </c>
+      <c r="E25" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" t="s">
+        <v>75</v>
+      </c>
+      <c r="E26" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
+        <v>78</v>
+      </c>
+      <c r="C27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" t="s">
+        <v>79</v>
+      </c>
+      <c r="E27" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" t="s">
+        <v>81</v>
+      </c>
+      <c r="E28" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>78</v>
+      </c>
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" t="s">
+        <v>84</v>
+      </c>
+      <c r="E29" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" t="s">
+        <v>85</v>
+      </c>
+      <c r="C30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" t="s">
+        <v>87</v>
+      </c>
+      <c r="E30" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" t="s">
+        <v>88</v>
+      </c>
+      <c r="C31" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" t="s">
+        <v>89</v>
+      </c>
+      <c r="E31" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32" t="s">
+        <v>91</v>
+      </c>
+      <c r="C32" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" t="s">
+        <v>92</v>
+      </c>
+      <c r="E32" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" t="s">
+        <v>93</v>
+      </c>
+      <c r="C33" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" t="s">
+        <v>94</v>
+      </c>
+      <c r="E33" t="s">
+        <v>95</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>